<commit_message>
excel_UE update for S4
</commit_message>
<xml_diff>
--- a/liens/excel_UE.xlsx
+++ b/liens/excel_UE.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomco\Documents\Ecole\2A\Secrétariat\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomco\Documents\Ecole\2A\S4\Secrétariat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F0D90A0-DF33-4E41-B60B-DE66B138C7B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D32F76C2-7F9A-4E96-8161-ECC370984A2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="45">
   <si>
     <t>Calcul des notes (BUT Infocom-Com' des Orgas) - savoir si les UE sont validées</t>
   </si>
@@ -72,9 +72,6 @@
     <t>Matière</t>
   </si>
   <si>
-    <t>TIC</t>
-  </si>
-  <si>
     <t>PPP</t>
   </si>
   <si>
@@ -132,71 +129,80 @@
     <t>Réussite</t>
   </si>
   <si>
-    <t>Culture numérique</t>
-  </si>
-  <si>
-    <t>Linguistique/sémio.</t>
-  </si>
-  <si>
     <t>Expression écr/orale</t>
   </si>
   <si>
-    <t>Conférences 40h</t>
-  </si>
-  <si>
-    <t>Conféren. heures maq.</t>
-  </si>
-  <si>
-    <t>Design graphique</t>
-  </si>
-  <si>
     <t>Gestion de projet</t>
   </si>
   <si>
-    <t>[Web]Marketing</t>
-  </si>
-  <si>
-    <t>Communication interne</t>
-  </si>
-  <si>
-    <t>Edition Web</t>
-  </si>
-  <si>
-    <t>Ecriture Pro.</t>
-  </si>
-  <si>
-    <t>Plan média</t>
-  </si>
-  <si>
-    <t>SAE concev. un éven.</t>
-  </si>
-  <si>
-    <t>SAE Projet éditorial</t>
-  </si>
-  <si>
-    <t>SAE recom. &amp; et. marché</t>
-  </si>
-  <si>
-    <t>SAE Création</t>
-  </si>
-  <si>
-    <t>SAE Etu. Marketing</t>
-  </si>
-  <si>
-    <t>SAE Portfolio</t>
-  </si>
-  <si>
     <t>Pourcentage</t>
   </si>
   <si>
     <t>Calcul des pourcentages de matières par rapport aux UE</t>
+  </si>
+  <si>
+    <t>SHS</t>
+  </si>
+  <si>
+    <t>Veille</t>
+  </si>
+  <si>
+    <t>Droit de l'Infocom'</t>
+  </si>
+  <si>
+    <t>Com' Numérique</t>
+  </si>
+  <si>
+    <t>Strat' de Com'</t>
+  </si>
+  <si>
+    <t>Edition de site web</t>
+  </si>
+  <si>
+    <t>Com' Publique</t>
+  </si>
+  <si>
+    <t>SAé Stage</t>
+  </si>
+  <si>
+    <t>SAé Portfolio</t>
+  </si>
+  <si>
+    <t>SAé Com' Numérique</t>
+  </si>
+  <si>
+    <t>Saé Réponse brief client</t>
+  </si>
+  <si>
+    <t>UE 4.1 - Décrypter</t>
+  </si>
+  <si>
+    <t>UE 4.2 - Partager</t>
+  </si>
+  <si>
+    <t>UE 4.3 - Concevoir une strat'</t>
+  </si>
+  <si>
+    <t>UE 4.4 - Elaborer des moyens</t>
+  </si>
+  <si>
+    <t>UE 4.5 - Piloter les relations</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Récapitulatif du poids de chaque matière en général</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="0.0%"/>
+  </numFmts>
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -260,6 +266,24 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -305,7 +329,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -616,36 +640,6 @@
         <color rgb="FF000000"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -665,13 +659,48 @@
     </border>
     <border>
       <left style="medium">
-        <color auto="1"/>
+        <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color auto="1"/>
+        <color rgb="FF000000"/>
       </right>
       <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
         <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
       </top>
       <bottom style="medium">
         <color auto="1"/>
@@ -680,13 +709,28 @@
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color auto="1"/>
+        <color rgb="FF000000"/>
       </right>
       <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
       </top>
       <bottom style="medium">
         <color auto="1"/>
@@ -703,8 +747,21 @@
       <top style="thin">
         <color auto="1"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom style="medium">
-        <color auto="1"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
@@ -712,7 +769,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -777,25 +834,16 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -825,6 +873,39 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -844,92 +925,95 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="4" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="8" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="8" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="14" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1148,8 +1232,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -1173,16 +1257,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A1" s="45" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
+      <c r="A1" s="53" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1">
       <c r="A2" s="1"/>
@@ -1195,22 +1279,22 @@
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="46"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="46"/>
-      <c r="K3" s="46"/>
-      <c r="L3" s="46"/>
-      <c r="M3" s="46"/>
-      <c r="N3" s="46"/>
+      <c r="B3" s="54"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="54"/>
+      <c r="H3" s="54"/>
+      <c r="I3" s="54"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="54"/>
+      <c r="L3" s="54"/>
+      <c r="M3" s="54"/>
+      <c r="N3" s="54"/>
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
@@ -1253,22 +1337,22 @@
       <c r="Z4" s="4"/>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A5" s="48" t="s">
+      <c r="A5" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="49"/>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="49"/>
-      <c r="H5" s="49"/>
-      <c r="I5" s="49"/>
-      <c r="J5" s="49"/>
-      <c r="K5" s="49"/>
-      <c r="L5" s="49"/>
-      <c r="M5" s="49"/>
-      <c r="N5" s="50"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="57"/>
+      <c r="F5" s="57"/>
+      <c r="G5" s="57"/>
+      <c r="H5" s="57"/>
+      <c r="I5" s="57"/>
+      <c r="J5" s="57"/>
+      <c r="K5" s="57"/>
+      <c r="L5" s="57"/>
+      <c r="M5" s="57"/>
+      <c r="N5" s="58"/>
       <c r="O5" s="5"/>
       <c r="P5" s="5"/>
       <c r="Q5" s="5"/>
@@ -1280,48 +1364,48 @@
         <v>3</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C6" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="F6" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="K6" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="K6" s="7" t="s">
-        <v>29</v>
-      </c>
       <c r="L6" s="7" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="N6" s="8" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
@@ -1347,32 +1431,20 @@
         <v>3</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="F8" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="G8" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="H8" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="I8" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="J8" s="15" t="s">
-        <v>41</v>
-      </c>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
       <c r="K8" s="15"/>
       <c r="L8" s="15"/>
       <c r="M8" s="15"/>
@@ -1385,7 +1457,7 @@
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" thickBot="1">
       <c r="A9" s="17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="18"/>
       <c r="C9" s="18"/>
@@ -1406,7 +1478,7 @@
       <c r="R9" s="13"/>
       <c r="S9" s="13"/>
     </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+    <row r="10" spans="1:26" ht="14.25" customHeight="1" thickBot="1">
       <c r="A10" s="22"/>
       <c r="B10" s="22"/>
       <c r="C10" s="22"/>
@@ -1416,1339 +1488,1352 @@
       <c r="G10" s="22"/>
       <c r="H10" s="22"/>
     </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A11" s="41" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="42"/>
-      <c r="C11" s="43"/>
-      <c r="E11" s="41" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="42"/>
-      <c r="G11" s="43"/>
-      <c r="I11" s="41" t="s">
-        <v>11</v>
-      </c>
-      <c r="J11" s="42"/>
-      <c r="K11" s="43"/>
-      <c r="M11" s="41" t="s">
-        <v>12</v>
-      </c>
-      <c r="N11" s="42"/>
-      <c r="O11" s="43"/>
-      <c r="Q11" s="41" t="s">
+    <row r="11" spans="1:26" ht="14.25" customHeight="1" thickBot="1">
+      <c r="A11" s="49" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="50"/>
+      <c r="C11" s="51"/>
+      <c r="E11" s="49" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" s="50"/>
+      <c r="G11" s="51"/>
+      <c r="I11" s="49" t="s">
+        <v>40</v>
+      </c>
+      <c r="J11" s="50"/>
+      <c r="K11" s="51"/>
+      <c r="M11" s="49" t="s">
+        <v>41</v>
+      </c>
+      <c r="N11" s="50"/>
+      <c r="O11" s="51"/>
+      <c r="Q11" s="49" t="s">
+        <v>42</v>
+      </c>
+      <c r="R11" s="50"/>
+      <c r="S11" s="51"/>
+    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" s="67" t="s">
         <v>13</v>
       </c>
-      <c r="R11" s="42"/>
-      <c r="S11" s="43"/>
-    </row>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A12" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="56" t="s">
+      <c r="B12" s="68" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="59" t="s">
-        <v>14</v>
-      </c>
-      <c r="F12" s="60" t="s">
+      <c r="C12" s="69" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="67" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" s="68" t="s">
         <v>3</v>
       </c>
-      <c r="G12" s="61" t="s">
-        <v>8</v>
-      </c>
-      <c r="I12" s="59" t="s">
-        <v>14</v>
-      </c>
-      <c r="J12" s="60" t="s">
+      <c r="G12" s="69" t="s">
+        <v>7</v>
+      </c>
+      <c r="I12" s="67" t="s">
+        <v>13</v>
+      </c>
+      <c r="J12" s="68" t="s">
         <v>3</v>
       </c>
-      <c r="K12" s="61" t="s">
-        <v>8</v>
-      </c>
-      <c r="M12" s="59" t="s">
-        <v>14</v>
-      </c>
-      <c r="N12" s="60" t="s">
+      <c r="K12" s="69" t="s">
+        <v>7</v>
+      </c>
+      <c r="M12" s="67" t="s">
+        <v>13</v>
+      </c>
+      <c r="N12" s="68" t="s">
         <v>3</v>
       </c>
-      <c r="O12" s="61" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q12" s="59" t="s">
-        <v>14</v>
-      </c>
-      <c r="R12" s="60" t="s">
+      <c r="O12" s="69" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q12" s="67" t="s">
+        <v>13</v>
+      </c>
+      <c r="R12" s="68" t="s">
         <v>3</v>
       </c>
-      <c r="S12" s="61" t="s">
-        <v>8</v>
+      <c r="S12" s="69" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A13" s="51">
-        <v>8</v>
+      <c r="A13" s="38">
+        <v>16</v>
       </c>
       <c r="B13" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="25">
+        <f>B7</f>
+        <v>0</v>
+      </c>
+      <c r="E13" s="24">
         <v>4</v>
       </c>
-      <c r="C13" s="26">
+      <c r="F13" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13" s="25">
         <f>C7</f>
         <v>0</v>
       </c>
-      <c r="E13" s="62">
-        <v>6</v>
-      </c>
-      <c r="F13" s="63" t="s">
-        <v>25</v>
-      </c>
-      <c r="G13" s="64">
-        <f>B$7</f>
-        <v>0</v>
-      </c>
-      <c r="I13" s="62">
-        <v>10</v>
-      </c>
-      <c r="J13" s="63" t="s">
-        <v>31</v>
-      </c>
-      <c r="K13" s="64">
-        <f>M7</f>
-        <v>0</v>
-      </c>
-      <c r="M13" s="25">
-        <v>12</v>
+      <c r="I13" s="24">
+        <v>4</v>
+      </c>
+      <c r="J13" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="K13" s="25">
+        <f>I7</f>
+        <v>0</v>
+      </c>
+      <c r="M13" s="24">
+        <v>24</v>
       </c>
       <c r="N13" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="O13" s="26">
-        <f>M7</f>
-        <v>0</v>
-      </c>
-      <c r="Q13" s="25">
-        <v>10</v>
+        <v>30</v>
+      </c>
+      <c r="O13" s="25">
+        <f>I7</f>
+        <v>0</v>
+      </c>
+      <c r="Q13" s="24">
+        <v>4</v>
       </c>
       <c r="R13" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="S13" s="26">
-        <f>L7</f>
+      <c r="S13" s="25">
+        <f>I7</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A14" s="51">
-        <v>8</v>
+      <c r="A14" s="38">
+        <v>6</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="26">
-        <f>B7</f>
-        <v>0</v>
-      </c>
-      <c r="E14" s="62">
-        <v>6</v>
-      </c>
-      <c r="F14" s="63" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="25">
+        <f>C7</f>
+        <v>0</v>
+      </c>
+      <c r="E14" s="24">
         <v>4</v>
       </c>
-      <c r="G14" s="64">
-        <f>C7</f>
-        <v>0</v>
-      </c>
-      <c r="I14" s="62">
-        <v>10</v>
-      </c>
-      <c r="J14" s="63" t="s">
-        <v>32</v>
-      </c>
-      <c r="K14" s="64">
-        <f>N7</f>
-        <v>0</v>
-      </c>
-      <c r="M14" s="25">
-        <v>10</v>
+      <c r="F14" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="G14" s="25">
+        <f>E7</f>
+        <v>0</v>
+      </c>
+      <c r="I14" s="24">
+        <v>16</v>
+      </c>
+      <c r="J14" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="K14" s="25">
+        <f>J7</f>
+        <v>0</v>
+      </c>
+      <c r="M14" s="24">
+        <v>12</v>
       </c>
       <c r="N14" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="O14" s="26">
+      <c r="O14" s="25">
+        <f>L7</f>
+        <v>0</v>
+      </c>
+      <c r="Q14" s="24">
+        <v>24</v>
+      </c>
+      <c r="R14" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="S14" s="25">
+        <f>K7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" s="38">
+        <v>8</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="25">
+        <f>D7</f>
+        <v>0</v>
+      </c>
+      <c r="E15" s="24">
+        <v>9</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="G15" s="25">
+        <f>F7</f>
+        <v>0</v>
+      </c>
+      <c r="I15" s="24">
+        <v>8</v>
+      </c>
+      <c r="J15" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="K15" s="25">
+        <f>L7</f>
+        <v>0</v>
+      </c>
+      <c r="M15" s="38">
+        <v>5</v>
+      </c>
+      <c r="N15" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="O15" s="25">
         <f>N7</f>
         <v>0</v>
       </c>
-      <c r="Q14" s="25">
-        <v>10</v>
-      </c>
-      <c r="R14" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="S14" s="26">
-        <f>M7</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A15" s="51">
+      <c r="Q15" s="24">
         <v>8</v>
-      </c>
-      <c r="B15" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="26">
-        <f>D7</f>
-        <v>0</v>
-      </c>
-      <c r="E15" s="62">
-        <v>6</v>
-      </c>
-      <c r="F15" s="63" t="s">
-        <v>24</v>
-      </c>
-      <c r="G15" s="64">
-        <f>D7</f>
-        <v>0</v>
-      </c>
-      <c r="I15" s="62">
-        <v>10</v>
-      </c>
-      <c r="J15" s="63" t="s">
-        <v>33</v>
-      </c>
-      <c r="K15" s="64">
-        <f>B9</f>
-        <v>0</v>
-      </c>
-      <c r="M15" s="25">
-        <v>10</v>
-      </c>
-      <c r="N15" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="O15" s="26">
-        <f>B9</f>
-        <v>0</v>
-      </c>
-      <c r="Q15" s="25">
-        <v>10</v>
       </c>
       <c r="R15" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="S15" s="26">
+      <c r="S15" s="25">
+        <f>L7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A16" s="38">
+        <v>6</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="25">
+        <f>E7</f>
+        <v>0</v>
+      </c>
+      <c r="E16" s="24">
+        <v>9</v>
+      </c>
+      <c r="F16" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="G16" s="25">
+        <f>G7</f>
+        <v>0</v>
+      </c>
+      <c r="I16" s="24">
+        <v>8</v>
+      </c>
+      <c r="J16" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="K16" s="25">
+        <f>M7</f>
+        <v>0</v>
+      </c>
+      <c r="M16" s="38">
+        <v>5</v>
+      </c>
+      <c r="N16" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="O16" s="25">
+        <f>$B$9</f>
+        <v>0</v>
+      </c>
+      <c r="Q16" s="38">
+        <v>5</v>
+      </c>
+      <c r="R16" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="S16" s="25">
         <f>N7</f>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A16" s="51">
-        <v>8</v>
-      </c>
-      <c r="B16" s="15" t="s">
+    <row r="17" spans="1:19" ht="14.25" customHeight="1">
+      <c r="A17" s="38">
         <v>5</v>
       </c>
-      <c r="C16" s="26">
-        <f>E7</f>
-        <v>0</v>
-      </c>
-      <c r="E16" s="62">
-        <v>2</v>
-      </c>
-      <c r="F16" s="63" t="s">
+      <c r="B17" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="25">
+        <f>N7</f>
+        <v>0</v>
+      </c>
+      <c r="E17" s="24">
+        <v>10</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="G17" s="25">
+        <f>H7</f>
+        <v>0</v>
+      </c>
+      <c r="I17" s="38">
         <v>5</v>
       </c>
-      <c r="G16" s="64">
-        <f>E7</f>
-        <v>0</v>
-      </c>
-      <c r="I16" s="62">
+      <c r="J17" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="K17" s="25">
+        <f>N7</f>
+        <v>0</v>
+      </c>
+      <c r="M17" s="38">
+        <v>4</v>
+      </c>
+      <c r="N17" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="O17" s="25">
+        <f>$C$9</f>
+        <v>0</v>
+      </c>
+      <c r="Q17" s="38">
+        <v>5</v>
+      </c>
+      <c r="R17" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="S17" s="25">
+        <f>$B$9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" ht="14.25" customHeight="1" thickBot="1">
+      <c r="A18" s="38">
+        <v>5</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="25">
+        <f>$B$9</f>
+        <v>0</v>
+      </c>
+      <c r="E18" s="38">
+        <v>5</v>
+      </c>
+      <c r="F18" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="G18" s="25">
+        <f>N7</f>
+        <v>0</v>
+      </c>
+      <c r="I18" s="38">
+        <v>5</v>
+      </c>
+      <c r="J18" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="K18" s="25">
+        <f>$B$9</f>
+        <v>0</v>
+      </c>
+      <c r="M18" s="42">
         <v>10</v>
       </c>
-      <c r="J16" s="63" t="s">
+      <c r="N18" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="K16" s="64">
-        <f>C9</f>
-        <v>0</v>
-      </c>
-      <c r="M16" s="25">
+      <c r="O18" s="40">
+        <f>$D$9</f>
+        <v>0</v>
+      </c>
+      <c r="Q18" s="38">
+        <v>4</v>
+      </c>
+      <c r="R18" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="S18" s="25">
+        <f>$C$9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" ht="14.25" customHeight="1" thickBot="1">
+      <c r="A19" s="38">
+        <v>4</v>
+      </c>
+      <c r="B19" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="25">
+        <f>$C$9</f>
+        <v>0</v>
+      </c>
+      <c r="E19" s="38">
+        <v>5</v>
+      </c>
+      <c r="F19" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="G19" s="25">
+        <f>$B$9</f>
+        <v>0</v>
+      </c>
+      <c r="I19" s="38">
+        <v>4</v>
+      </c>
+      <c r="J19" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="K19" s="25">
+        <f>$C$9</f>
+        <v>0</v>
+      </c>
+      <c r="M19" s="62"/>
+      <c r="N19" s="62"/>
+      <c r="O19" s="65"/>
+      <c r="Q19" s="42">
         <v>10</v>
       </c>
-      <c r="N16" s="15" t="s">
+      <c r="R19" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="O16" s="26">
-        <f>C9</f>
-        <v>0</v>
-      </c>
-      <c r="Q16" s="25">
+      <c r="S19" s="40">
+        <f>$D$9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" ht="14.25" customHeight="1" thickBot="1">
+      <c r="A20" s="42">
         <v>10</v>
       </c>
-      <c r="R16" s="15" t="s">
+      <c r="B20" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="40">
+        <f>$D$9</f>
+        <v>0</v>
+      </c>
+      <c r="E20" s="38">
+        <v>4</v>
+      </c>
+      <c r="F20" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="S16" s="26">
-        <f>D9</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" ht="14.25" customHeight="1">
-      <c r="A17" s="51">
-        <v>2</v>
-      </c>
-      <c r="B17" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" s="26">
-        <f>L7</f>
-        <v>0</v>
-      </c>
-      <c r="E17" s="62">
-        <v>6</v>
-      </c>
-      <c r="F17" s="63" t="s">
-        <v>6</v>
-      </c>
-      <c r="G17" s="64">
-        <f>F7</f>
-        <v>0</v>
-      </c>
-      <c r="I17" s="62">
-        <v>6</v>
-      </c>
-      <c r="J17" s="63" t="s">
-        <v>37</v>
-      </c>
-      <c r="K17" s="64">
-        <f>G9</f>
-        <v>0</v>
-      </c>
-      <c r="M17" s="25">
-        <v>4</v>
-      </c>
-      <c r="N17" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="O17" s="26">
-        <f>E9</f>
-        <v>0</v>
-      </c>
-      <c r="Q17" s="25">
-        <v>6</v>
-      </c>
-      <c r="R17" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="S17" s="26">
-        <f>F9</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" ht="14.25" customHeight="1">
-      <c r="A18" s="51">
-        <v>2</v>
-      </c>
-      <c r="B18" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="C18" s="26">
-        <f>N7</f>
-        <v>0</v>
-      </c>
-      <c r="E18" s="62">
-        <v>6</v>
-      </c>
-      <c r="F18" s="63" t="s">
-        <v>7</v>
-      </c>
-      <c r="G18" s="64">
-        <f>G7</f>
-        <v>0</v>
-      </c>
-      <c r="I18" s="62">
-        <v>6</v>
-      </c>
-      <c r="J18" s="70" t="s">
-        <v>39</v>
-      </c>
-      <c r="K18" s="64">
-        <f>H9</f>
-        <v>0</v>
-      </c>
-      <c r="M18" s="25">
-        <v>2</v>
-      </c>
-      <c r="N18" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="O18" s="26">
-        <f>G9</f>
-        <v>0</v>
-      </c>
-      <c r="Q18" s="25">
-        <v>4</v>
-      </c>
-      <c r="R18" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="S18" s="26">
-        <f>G9</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19" ht="14.25" customHeight="1">
-      <c r="A19" s="51">
-        <v>2</v>
-      </c>
-      <c r="B19" s="15" t="s">
+      <c r="G20" s="25">
+        <f>$C$9</f>
+        <v>0</v>
+      </c>
+      <c r="I20" s="42">
+        <v>10</v>
+      </c>
+      <c r="J20" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="C19" s="30">
-        <f>C9</f>
-        <v>0</v>
-      </c>
-      <c r="E19" s="62">
-        <v>6</v>
-      </c>
-      <c r="F19" s="63" t="s">
-        <v>26</v>
-      </c>
-      <c r="G19" s="64">
-        <f>H7</f>
-        <v>0</v>
-      </c>
-      <c r="I19" s="62">
-        <v>4</v>
-      </c>
-      <c r="J19" s="63" t="s">
-        <v>40</v>
-      </c>
-      <c r="K19" s="64">
-        <f>I9</f>
-        <v>0</v>
-      </c>
-      <c r="M19" s="25">
-        <v>4</v>
-      </c>
-      <c r="N19" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="O19" s="73">
-        <f>H9</f>
-        <v>0</v>
-      </c>
-      <c r="Q19" s="25">
-        <v>6</v>
-      </c>
-      <c r="R19" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="S19" s="54">
-        <f>H9</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A20" s="57">
-        <v>4</v>
-      </c>
-      <c r="B20" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="C20" s="54">
-        <f>E9</f>
-        <v>0</v>
-      </c>
-      <c r="E20" s="62">
-        <v>2</v>
-      </c>
-      <c r="F20" s="63" t="s">
+      <c r="K20" s="40">
+        <f>$D$9</f>
+        <v>0</v>
+      </c>
+      <c r="M20" s="63"/>
+      <c r="N20" s="63"/>
+      <c r="O20" s="66"/>
+      <c r="Q20" s="62"/>
+      <c r="R20" s="62"/>
+      <c r="S20" s="62"/>
+    </row>
+    <row r="21" spans="1:19" ht="14.25" customHeight="1" thickBot="1">
+      <c r="A21" s="62"/>
+      <c r="B21" s="62"/>
+      <c r="C21" s="62"/>
+      <c r="E21" s="70">
+        <v>10</v>
+      </c>
+      <c r="F21" s="71" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="65">
-        <f>C9</f>
-        <v>0</v>
-      </c>
-      <c r="I20" s="71">
-        <v>4</v>
-      </c>
-      <c r="J20" s="72" t="s">
-        <v>41</v>
-      </c>
-      <c r="K20" s="69">
-        <f>J9</f>
-        <v>0</v>
-      </c>
-      <c r="M20" s="25">
-        <v>4</v>
-      </c>
-      <c r="N20" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="O20" s="73">
-        <f>I9</f>
-        <v>0</v>
-      </c>
-      <c r="Q20" s="27">
-        <v>4</v>
-      </c>
-      <c r="R20" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="S20" s="55">
-        <f>J9</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A21" s="57">
-        <v>6</v>
-      </c>
-      <c r="B21" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="C21" s="54">
-        <f>F9</f>
-        <v>0</v>
-      </c>
-      <c r="E21" s="62">
-        <v>6</v>
-      </c>
-      <c r="F21" s="63" t="s">
-        <v>36</v>
-      </c>
-      <c r="G21" s="66">
-        <f>E9</f>
-        <v>0</v>
-      </c>
-      <c r="I21" s="31"/>
-      <c r="K21" s="31"/>
-      <c r="M21" s="27">
-        <v>4</v>
-      </c>
-      <c r="N21" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="O21" s="74">
-        <f>J9</f>
-        <v>0</v>
-      </c>
+      <c r="G21" s="72">
+        <f>$D$9</f>
+        <v>0</v>
+      </c>
+      <c r="I21" s="28"/>
+      <c r="K21" s="28"/>
+      <c r="M21" s="63"/>
+      <c r="N21" s="63"/>
+      <c r="O21" s="66"/>
     </row>
     <row r="22" spans="1:19" ht="14.25" customHeight="1">
-      <c r="A22" s="57">
-        <v>6</v>
-      </c>
-      <c r="B22" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="C22" s="54">
-        <f>G9</f>
-        <v>0</v>
-      </c>
-      <c r="E22" s="62">
-        <v>6</v>
-      </c>
-      <c r="F22" s="63" t="s">
-        <v>38</v>
-      </c>
-      <c r="G22" s="66">
-        <f>F9</f>
-        <v>0</v>
-      </c>
-      <c r="I22" s="31"/>
-      <c r="J22" s="31"/>
-      <c r="K22" s="31"/>
-    </row>
-    <row r="23" spans="1:19" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A23" s="58">
-        <v>6</v>
-      </c>
-      <c r="B23" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="C23" s="55">
-        <f>J9</f>
-        <v>0</v>
-      </c>
-      <c r="E23" s="62">
-        <v>4</v>
-      </c>
-      <c r="F23" s="63" t="s">
-        <v>37</v>
-      </c>
-      <c r="G23" s="66">
-        <f>G9</f>
-        <v>0</v>
-      </c>
-      <c r="I23" s="31"/>
-      <c r="J23" s="31"/>
-      <c r="K23" s="31"/>
-    </row>
-    <row r="24" spans="1:19" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A24" s="31"/>
-      <c r="B24" s="53"/>
-      <c r="C24" s="31"/>
-      <c r="E24" s="67">
-        <v>4</v>
-      </c>
-      <c r="F24" s="68" t="s">
-        <v>41</v>
-      </c>
-      <c r="G24" s="69">
-        <f>J9</f>
-        <v>0</v>
-      </c>
-      <c r="I24" s="31"/>
-      <c r="J24" s="31"/>
-      <c r="K24" s="31"/>
+      <c r="A22" s="63"/>
+      <c r="B22" s="63"/>
+      <c r="C22" s="63"/>
+      <c r="E22" s="64"/>
+      <c r="F22" s="64"/>
+      <c r="G22" s="64"/>
+      <c r="I22" s="28"/>
+      <c r="J22" s="28"/>
+      <c r="K22" s="28"/>
+    </row>
+    <row r="23" spans="1:19" ht="14.25" customHeight="1">
+      <c r="A23" s="63"/>
+      <c r="B23" s="63"/>
+      <c r="C23" s="63"/>
+      <c r="E23" s="63"/>
+      <c r="F23" s="63"/>
+      <c r="G23" s="63"/>
+      <c r="I23" s="28"/>
+      <c r="J23" s="28"/>
+      <c r="K23" s="28"/>
+    </row>
+    <row r="24" spans="1:19" ht="14.25" customHeight="1">
+      <c r="A24" s="28"/>
+      <c r="B24" s="28"/>
+      <c r="C24" s="28"/>
+      <c r="E24" s="63"/>
+      <c r="F24" s="63"/>
+      <c r="G24" s="63"/>
+      <c r="I24" s="28"/>
+      <c r="J24" s="28"/>
+      <c r="K24" s="28"/>
     </row>
     <row r="25" spans="1:19" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A25" s="31"/>
-      <c r="B25" s="31"/>
-      <c r="C25" s="31"/>
+      <c r="A25" s="28"/>
+      <c r="B25" s="28"/>
+      <c r="C25" s="28"/>
     </row>
     <row r="26" spans="1:19" ht="14.25" customHeight="1">
-      <c r="A26" s="44" t="s">
+      <c r="A26" s="52" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26" s="50"/>
+      <c r="C26" s="50"/>
+      <c r="D26" s="50"/>
+      <c r="E26" s="50"/>
+      <c r="F26" s="51"/>
+    </row>
+    <row r="27" spans="1:19" ht="14.25" customHeight="1">
+      <c r="A27" s="29"/>
+      <c r="B27" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="B26" s="42"/>
-      <c r="C26" s="42"/>
-      <c r="D26" s="42"/>
-      <c r="E26" s="42"/>
-      <c r="F26" s="43"/>
-    </row>
-    <row r="27" spans="1:19" ht="14.25" customHeight="1">
-      <c r="A27" s="32"/>
-      <c r="B27" s="33" t="s">
+      <c r="C27" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="C27" s="33" t="s">
+      <c r="D27" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="D27" s="33" t="s">
+      <c r="E27" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="E27" s="33" t="s">
+      <c r="F27" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="F27" s="34" t="s">
+    </row>
+    <row r="28" spans="1:19" ht="14.25" customHeight="1">
+      <c r="A28" s="32" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="28" spans="1:19" ht="14.25" customHeight="1">
-      <c r="A28" s="35" t="s">
-        <v>21</v>
-      </c>
-      <c r="B28" s="36">
+      <c r="B28" s="33">
         <f>SUM(A13:A23)</f>
         <v>60</v>
       </c>
-      <c r="C28" s="36">
+      <c r="C28" s="33">
         <f>SUM(E13:E24)</f>
         <v>60</v>
       </c>
-      <c r="D28" s="36">
+      <c r="D28" s="33">
         <f>SUM(I13:I20)</f>
         <v>60</v>
       </c>
-      <c r="E28" s="36">
+      <c r="E28" s="33">
         <f>SUM(M13:M21)</f>
         <v>60</v>
       </c>
-      <c r="F28" s="26">
+      <c r="F28" s="25">
         <f>SUM(Q13:Q20)</f>
         <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:19" ht="14.25" customHeight="1">
-      <c r="A29" s="35" t="s">
+      <c r="A29" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="B29" s="33" cm="1">
+        <f t="array" ref="B29">SUM(C13:C23*A13:A23/B28)</f>
+        <v>0</v>
+      </c>
+      <c r="C29" s="33" cm="1">
+        <f t="array" ref="C29">SUM(G13:G24*E13:E24/C28)</f>
+        <v>0</v>
+      </c>
+      <c r="D29" s="33" cm="1">
+        <f t="array" ref="D29">SUM(K13:K20*I13:I20/D28)</f>
+        <v>0</v>
+      </c>
+      <c r="E29" s="34" cm="1">
+        <f t="array" ref="E29">SUM(O13:O21*M13:M21/D28)</f>
+        <v>0</v>
+      </c>
+      <c r="F29" s="25" cm="1">
+        <f t="array" ref="F29">SUM(S13:S20*Q13:Q20/D28)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" ht="14.25" customHeight="1">
+      <c r="A30" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="B29" s="36" cm="1">
-        <f t="array" ref="B29">SUM(C13:C23*A13:A23/B28)</f>
-        <v>0</v>
-      </c>
-      <c r="C29" s="36" cm="1">
-        <f t="array" ref="C29">SUM(G13:G24*E13:E24/C28)</f>
-        <v>0</v>
-      </c>
-      <c r="D29" s="36" cm="1">
-        <f t="array" ref="D29">SUM(K13:K20*I13:I20/D28)</f>
-        <v>0</v>
-      </c>
-      <c r="E29" s="37" cm="1">
-        <f t="array" ref="E29">SUM(O13:O21*M13:M21/D28)</f>
-        <v>0</v>
-      </c>
-      <c r="F29" s="26" cm="1">
-        <f t="array" ref="F29">SUM(S13:S20*Q13:Q20/D28)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:19" ht="14.25" customHeight="1">
-      <c r="A30" s="38" t="s">
-        <v>23</v>
-      </c>
-      <c r="B30" s="39" t="str">
+      <c r="B30" s="36" t="str">
         <f t="shared" ref="B30:F30" si="0">IF(B29&lt;10,"Non","Oui")</f>
         <v>Non</v>
       </c>
-      <c r="C30" s="39" t="str">
+      <c r="C30" s="36" t="str">
         <f>IF(C29&lt;10,"Non","Oui")</f>
         <v>Non</v>
       </c>
-      <c r="D30" s="39" t="str">
+      <c r="D30" s="36" t="str">
         <f t="shared" si="0"/>
         <v>Non</v>
       </c>
-      <c r="E30" s="39" t="str">
+      <c r="E30" s="36" t="str">
         <f t="shared" si="0"/>
         <v>Non</v>
       </c>
-      <c r="F30" s="29" t="str">
+      <c r="F30" s="27" t="str">
         <f t="shared" si="0"/>
         <v>Non</v>
       </c>
     </row>
     <row r="31" spans="1:19" ht="14.25" customHeight="1">
-      <c r="A31" s="31"/>
-      <c r="B31" s="40"/>
-      <c r="C31" s="31"/>
+      <c r="A31" s="28"/>
+      <c r="B31" s="37"/>
+      <c r="C31" s="28"/>
     </row>
     <row r="32" spans="1:19" ht="14.25" customHeight="1">
-      <c r="A32" s="79" t="s">
-        <v>43</v>
-      </c>
-      <c r="B32" s="46"/>
-      <c r="C32" s="46"/>
-      <c r="D32" s="46"/>
-      <c r="E32" s="46"/>
-      <c r="F32" s="46"/>
-      <c r="G32" s="46"/>
-      <c r="H32" s="46"/>
+      <c r="A32" s="59" t="s">
+        <v>26</v>
+      </c>
+      <c r="B32" s="54"/>
+      <c r="C32" s="54"/>
+      <c r="D32" s="54"/>
+      <c r="E32" s="54"/>
+      <c r="F32" s="54"/>
+      <c r="G32" s="54"/>
+      <c r="H32" s="54"/>
     </row>
     <row r="33" spans="1:19" ht="14.25" customHeight="1" thickBot="1">
-      <c r="D33" s="31"/>
+      <c r="D33" s="28"/>
     </row>
     <row r="34" spans="1:19" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A34" s="41" t="s">
+      <c r="A34" s="49" t="s">
+        <v>8</v>
+      </c>
+      <c r="B34" s="50"/>
+      <c r="C34" s="51"/>
+      <c r="E34" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="B34" s="42"/>
-      <c r="C34" s="43"/>
-      <c r="E34" s="41" t="s">
+      <c r="F34" s="50"/>
+      <c r="G34" s="51"/>
+      <c r="I34" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="F34" s="42"/>
-      <c r="G34" s="43"/>
-      <c r="I34" s="41" t="s">
+      <c r="J34" s="50"/>
+      <c r="K34" s="51"/>
+      <c r="M34" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="J34" s="42"/>
-      <c r="K34" s="43"/>
-      <c r="M34" s="41" t="s">
+      <c r="N34" s="50"/>
+      <c r="O34" s="51"/>
+      <c r="Q34" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="N34" s="42"/>
-      <c r="O34" s="43"/>
-      <c r="Q34" s="41" t="s">
-        <v>13</v>
-      </c>
-      <c r="R34" s="42"/>
-      <c r="S34" s="43"/>
+      <c r="R34" s="50"/>
+      <c r="S34" s="51"/>
     </row>
     <row r="35" spans="1:19" ht="14.25" customHeight="1">
       <c r="A35" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="B35" s="56" t="s">
+        <v>13</v>
+      </c>
+      <c r="B35" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="C35" s="75" t="s">
-        <v>42</v>
-      </c>
-      <c r="E35" s="59" t="s">
-        <v>14</v>
-      </c>
-      <c r="F35" s="60" t="s">
+      <c r="C35" s="45" t="s">
+        <v>25</v>
+      </c>
+      <c r="E35" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="F35" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="G35" s="75" t="s">
-        <v>42</v>
-      </c>
-      <c r="I35" s="59" t="s">
-        <v>14</v>
-      </c>
-      <c r="J35" s="60" t="s">
+      <c r="G35" s="45" t="s">
+        <v>25</v>
+      </c>
+      <c r="I35" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="J35" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="K35" s="75" t="s">
-        <v>42</v>
-      </c>
-      <c r="M35" s="59" t="s">
-        <v>14</v>
-      </c>
-      <c r="N35" s="60" t="s">
+      <c r="K35" s="45" t="s">
+        <v>25</v>
+      </c>
+      <c r="M35" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="N35" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="O35" s="75" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q35" s="59" t="s">
-        <v>14</v>
-      </c>
-      <c r="R35" s="60" t="s">
+      <c r="O35" s="45" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q35" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="R35" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="S35" s="76" t="s">
-        <v>42</v>
+      <c r="S35" s="46" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="36" spans="1:19" ht="14.25" customHeight="1">
-      <c r="A36" s="51">
-        <v>8</v>
+      <c r="A36" s="38">
+        <v>16</v>
       </c>
       <c r="B36" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C36" s="47">
+        <f>$A36/$B$28</f>
+        <v>0.26666666666666666</v>
+      </c>
+      <c r="E36" s="24">
         <v>4</v>
       </c>
-      <c r="C36" s="77">
-        <f>$A36/$B$28</f>
-        <v>0.13333333333333333</v>
-      </c>
-      <c r="E36" s="62">
-        <v>6</v>
-      </c>
-      <c r="F36" s="63" t="s">
-        <v>25</v>
-      </c>
-      <c r="G36" s="78">
+      <c r="F36" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="G36" s="48">
         <f>$E36/$C$28</f>
-        <v>0.1</v>
-      </c>
-      <c r="I36" s="62">
-        <v>10</v>
-      </c>
-      <c r="J36" s="63" t="s">
-        <v>31</v>
-      </c>
-      <c r="K36" s="78">
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="I36" s="24">
+        <v>4</v>
+      </c>
+      <c r="J36" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="K36" s="48">
         <f>$I36/$D$28</f>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="M36" s="25">
-        <v>12</v>
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="M36" s="24">
+        <v>24</v>
       </c>
       <c r="N36" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="O36" s="77">
+        <v>30</v>
+      </c>
+      <c r="O36" s="47">
         <f>$M36/$E$28</f>
-        <v>0.2</v>
-      </c>
-      <c r="Q36" s="25">
-        <v>10</v>
+        <v>0.4</v>
+      </c>
+      <c r="Q36" s="24">
+        <v>4</v>
       </c>
       <c r="R36" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="S36" s="77">
+      <c r="S36" s="47">
         <f>$Q36/$F$28</f>
-        <v>0.16666666666666666</v>
+        <v>6.6666666666666666E-2</v>
       </c>
     </row>
     <row r="37" spans="1:19" ht="14.25" customHeight="1">
-      <c r="A37" s="51">
-        <v>8</v>
+      <c r="A37" s="38">
+        <v>6</v>
       </c>
       <c r="B37" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C37" s="77">
+        <v>29</v>
+      </c>
+      <c r="C37" s="47">
         <f t="shared" ref="C37:C46" si="1">$A37/$B$28</f>
-        <v>0.13333333333333333</v>
-      </c>
-      <c r="E37" s="62">
-        <v>6</v>
-      </c>
-      <c r="F37" s="63" t="s">
+        <v>0.1</v>
+      </c>
+      <c r="E37" s="24">
         <v>4</v>
       </c>
-      <c r="G37" s="78">
+      <c r="F37" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="G37" s="48">
         <f t="shared" ref="G37:G47" si="2">$E37/$C$28</f>
-        <v>0.1</v>
-      </c>
-      <c r="I37" s="62">
-        <v>10</v>
-      </c>
-      <c r="J37" s="63" t="s">
-        <v>32</v>
-      </c>
-      <c r="K37" s="78">
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="I37" s="24">
+        <v>16</v>
+      </c>
+      <c r="J37" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="K37" s="48">
         <f t="shared" ref="K37:K42" si="3">$I37/$D$28</f>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="M37" s="25">
-        <v>10</v>
+        <v>0.26666666666666666</v>
+      </c>
+      <c r="M37" s="24">
+        <v>12</v>
       </c>
       <c r="N37" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="O37" s="77">
+      <c r="O37" s="47">
         <f t="shared" ref="O37:O44" si="4">$M37/$E$28</f>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="Q37" s="25">
-        <v>10</v>
+        <v>0.2</v>
+      </c>
+      <c r="Q37" s="24">
+        <v>24</v>
       </c>
       <c r="R37" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="S37" s="77">
+        <v>24</v>
+      </c>
+      <c r="S37" s="47">
         <f t="shared" ref="S37:S43" si="5">$Q37/$F$28</f>
-        <v>0.16666666666666666</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="38" spans="1:19" ht="14.25" customHeight="1">
-      <c r="A38" s="51">
+      <c r="A38" s="38">
         <v>8</v>
       </c>
       <c r="B38" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C38" s="77">
+        <v>28</v>
+      </c>
+      <c r="C38" s="47">
         <f t="shared" si="1"/>
         <v>0.13333333333333333</v>
       </c>
-      <c r="E38" s="62">
+      <c r="E38" s="24">
+        <v>9</v>
+      </c>
+      <c r="F38" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="G38" s="48">
+        <f t="shared" si="2"/>
+        <v>0.15</v>
+      </c>
+      <c r="I38" s="24">
+        <v>8</v>
+      </c>
+      <c r="J38" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="K38" s="48">
+        <f t="shared" si="3"/>
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="M38" s="38">
+        <v>5</v>
+      </c>
+      <c r="N38" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="O38" s="47">
+        <f t="shared" si="4"/>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="Q38" s="24">
+        <v>8</v>
+      </c>
+      <c r="R38" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="S38" s="47">
+        <f t="shared" si="5"/>
+        <v>0.13333333333333333</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" ht="14.25" customHeight="1">
+      <c r="A39" s="38">
         <v>6</v>
       </c>
-      <c r="F38" s="63" t="s">
-        <v>24</v>
-      </c>
-      <c r="G38" s="78">
+      <c r="B39" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C39" s="47">
+        <f t="shared" si="1"/>
+        <v>0.1</v>
+      </c>
+      <c r="E39" s="24">
+        <v>9</v>
+      </c>
+      <c r="F39" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="G39" s="48">
         <f t="shared" si="2"/>
-        <v>0.1</v>
-      </c>
-      <c r="I38" s="62">
+        <v>0.15</v>
+      </c>
+      <c r="I39" s="24">
+        <v>8</v>
+      </c>
+      <c r="J39" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="K39" s="48">
+        <f t="shared" si="3"/>
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="M39" s="38">
+        <v>5</v>
+      </c>
+      <c r="N39" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="O39" s="47">
+        <f t="shared" si="4"/>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="Q39" s="38">
+        <v>5</v>
+      </c>
+      <c r="R39" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="S39" s="47">
+        <f t="shared" si="5"/>
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" ht="14.25" customHeight="1">
+      <c r="A40" s="38">
+        <v>5</v>
+      </c>
+      <c r="B40" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C40" s="47">
+        <f t="shared" si="1"/>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="E40" s="24">
         <v>10</v>
       </c>
-      <c r="J38" s="63" t="s">
-        <v>33</v>
-      </c>
-      <c r="K38" s="78">
+      <c r="F40" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="G40" s="48">
+        <f t="shared" si="2"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I40" s="38">
+        <v>5</v>
+      </c>
+      <c r="J40" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="K40" s="48">
         <f t="shared" si="3"/>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="M38" s="25">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="M40" s="38">
+        <v>4</v>
+      </c>
+      <c r="N40" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="O40" s="47">
+        <f t="shared" si="4"/>
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="Q40" s="38">
+        <v>5</v>
+      </c>
+      <c r="R40" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="S40" s="47">
+        <f t="shared" si="5"/>
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" ht="14.25" customHeight="1" thickBot="1">
+      <c r="A41" s="38">
+        <v>5</v>
+      </c>
+      <c r="B41" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C41" s="47">
+        <f t="shared" si="1"/>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="E41" s="38">
+        <v>5</v>
+      </c>
+      <c r="F41" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="G41" s="48">
+        <f t="shared" si="2"/>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="I41" s="38">
+        <v>5</v>
+      </c>
+      <c r="J41" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="K41" s="48">
+        <f t="shared" si="3"/>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="M41" s="60">
         <v>10</v>
       </c>
-      <c r="N38" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="O38" s="77">
+      <c r="N41" s="61" t="s">
+        <v>34</v>
+      </c>
+      <c r="O41" s="73">
         <f t="shared" si="4"/>
         <v>0.16666666666666666</v>
       </c>
-      <c r="Q38" s="25">
+      <c r="Q41" s="38">
+        <v>4</v>
+      </c>
+      <c r="R41" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="S41" s="47">
+        <f t="shared" si="5"/>
+        <v>6.6666666666666666E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" ht="14.25" customHeight="1" thickBot="1">
+      <c r="A42" s="38">
+        <v>4</v>
+      </c>
+      <c r="B42" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="C42" s="47">
+        <f t="shared" si="1"/>
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="E42" s="38">
+        <v>5</v>
+      </c>
+      <c r="F42" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="G42" s="48">
+        <f t="shared" si="2"/>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="I42" s="38">
+        <v>4</v>
+      </c>
+      <c r="J42" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="K42" s="48">
+        <f t="shared" si="3"/>
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="M42" s="78" t="s">
+        <v>43</v>
+      </c>
+      <c r="N42" s="62"/>
+      <c r="O42" s="74"/>
+      <c r="Q42" s="60">
         <v>10</v>
       </c>
-      <c r="R38" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="S38" s="77">
+      <c r="R42" s="61" t="s">
+        <v>34</v>
+      </c>
+      <c r="S42" s="73">
         <f t="shared" si="5"/>
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="39" spans="1:19" ht="14.25" customHeight="1">
-      <c r="A39" s="51">
-        <v>8</v>
-      </c>
-      <c r="B39" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C39" s="77">
+    <row r="43" spans="1:19" ht="14.25" customHeight="1" thickBot="1">
+      <c r="A43" s="60">
+        <v>10</v>
+      </c>
+      <c r="B43" s="61" t="s">
+        <v>34</v>
+      </c>
+      <c r="C43" s="73">
         <f t="shared" si="1"/>
-        <v>0.13333333333333333</v>
-      </c>
-      <c r="E39" s="62">
-        <v>2</v>
-      </c>
-      <c r="F39" s="63" t="s">
-        <v>5</v>
-      </c>
-      <c r="G39" s="78">
-        <f t="shared" si="2"/>
-        <v>3.3333333333333333E-2</v>
-      </c>
-      <c r="I39" s="62">
-        <v>10</v>
-      </c>
-      <c r="J39" s="63" t="s">
-        <v>34</v>
-      </c>
-      <c r="K39" s="78">
-        <f t="shared" si="3"/>
         <v>0.16666666666666666</v>
       </c>
-      <c r="M39" s="25">
-        <v>10</v>
-      </c>
-      <c r="N39" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="O39" s="77">
-        <f t="shared" si="4"/>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="Q39" s="25">
-        <v>10</v>
-      </c>
-      <c r="R39" s="15" t="s">
+      <c r="E43" s="38">
+        <v>4</v>
+      </c>
+      <c r="F43" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="S39" s="77">
-        <f t="shared" si="5"/>
-        <v>0.16666666666666666</v>
-      </c>
-    </row>
-    <row r="40" spans="1:19" ht="14.25" customHeight="1">
-      <c r="A40" s="51">
-        <v>2</v>
-      </c>
-      <c r="B40" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="C40" s="77">
-        <f t="shared" si="1"/>
-        <v>3.3333333333333333E-2</v>
-      </c>
-      <c r="E40" s="62">
-        <v>6</v>
-      </c>
-      <c r="F40" s="63" t="s">
-        <v>6</v>
-      </c>
-      <c r="G40" s="78">
-        <f t="shared" si="2"/>
-        <v>0.1</v>
-      </c>
-      <c r="I40" s="62">
-        <v>6</v>
-      </c>
-      <c r="J40" s="63" t="s">
-        <v>37</v>
-      </c>
-      <c r="K40" s="78">
-        <f t="shared" si="3"/>
-        <v>0.1</v>
-      </c>
-      <c r="M40" s="25">
-        <v>4</v>
-      </c>
-      <c r="N40" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="O40" s="77">
-        <f t="shared" si="4"/>
-        <v>6.6666666666666666E-2</v>
-      </c>
-      <c r="Q40" s="25">
-        <v>6</v>
-      </c>
-      <c r="R40" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="S40" s="77">
-        <f t="shared" si="5"/>
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:19" ht="14.25" customHeight="1">
-      <c r="A41" s="51">
-        <v>2</v>
-      </c>
-      <c r="B41" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="C41" s="77">
-        <f t="shared" si="1"/>
-        <v>3.3333333333333333E-2</v>
-      </c>
-      <c r="E41" s="62">
-        <v>6</v>
-      </c>
-      <c r="F41" s="63" t="s">
-        <v>7</v>
-      </c>
-      <c r="G41" s="78">
-        <f t="shared" si="2"/>
-        <v>0.1</v>
-      </c>
-      <c r="I41" s="62">
-        <v>6</v>
-      </c>
-      <c r="J41" s="70" t="s">
-        <v>39</v>
-      </c>
-      <c r="K41" s="78">
-        <f t="shared" si="3"/>
-        <v>0.1</v>
-      </c>
-      <c r="M41" s="25">
-        <v>2</v>
-      </c>
-      <c r="N41" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="O41" s="77">
-        <f t="shared" si="4"/>
-        <v>3.3333333333333333E-2</v>
-      </c>
-      <c r="Q41" s="25">
-        <v>4</v>
-      </c>
-      <c r="R41" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="S41" s="77">
-        <f t="shared" si="5"/>
-        <v>6.6666666666666666E-2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:19" ht="14.25" customHeight="1">
-      <c r="A42" s="51">
-        <v>2</v>
-      </c>
-      <c r="B42" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="C42" s="77">
-        <f t="shared" si="1"/>
-        <v>3.3333333333333333E-2</v>
-      </c>
-      <c r="E42" s="62">
-        <v>6</v>
-      </c>
-      <c r="F42" s="63" t="s">
-        <v>26</v>
-      </c>
-      <c r="G42" s="78">
-        <f t="shared" si="2"/>
-        <v>0.1</v>
-      </c>
-      <c r="I42" s="62">
-        <v>4</v>
-      </c>
-      <c r="J42" s="63" t="s">
-        <v>40</v>
-      </c>
-      <c r="K42" s="78">
-        <f t="shared" si="3"/>
-        <v>6.6666666666666666E-2</v>
-      </c>
-      <c r="M42" s="25">
-        <v>4</v>
-      </c>
-      <c r="N42" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="O42" s="77">
-        <f t="shared" si="4"/>
-        <v>6.6666666666666666E-2</v>
-      </c>
-      <c r="Q42" s="25">
-        <v>6</v>
-      </c>
-      <c r="R42" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="S42" s="77">
-        <f t="shared" si="5"/>
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:19" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A43" s="57">
-        <v>4</v>
-      </c>
-      <c r="B43" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="C43" s="77">
-        <f t="shared" si="1"/>
-        <v>6.6666666666666666E-2</v>
-      </c>
-      <c r="E43" s="62">
-        <v>2</v>
-      </c>
-      <c r="F43" s="63" t="s">
-        <v>34</v>
-      </c>
-      <c r="G43" s="78">
-        <f t="shared" si="2"/>
-        <v>3.3333333333333333E-2</v>
-      </c>
-      <c r="I43" s="71">
-        <v>4</v>
-      </c>
-      <c r="J43" s="72" t="s">
-        <v>41</v>
-      </c>
-      <c r="K43" s="78">
-        <f>$I43/$D$28</f>
-        <v>6.6666666666666666E-2</v>
-      </c>
-      <c r="M43" s="25">
-        <v>4</v>
-      </c>
-      <c r="N43" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="O43" s="77">
-        <f t="shared" si="4"/>
-        <v>6.6666666666666666E-2</v>
-      </c>
-      <c r="Q43" s="27">
-        <v>4</v>
-      </c>
-      <c r="R43" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="S43" s="77">
-        <f t="shared" si="5"/>
-        <v>6.6666666666666666E-2</v>
-      </c>
-    </row>
-    <row r="44" spans="1:19" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A44" s="57">
-        <v>6</v>
-      </c>
-      <c r="B44" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="C44" s="77">
-        <f t="shared" si="1"/>
-        <v>0.1</v>
-      </c>
-      <c r="E44" s="62">
-        <v>6</v>
-      </c>
-      <c r="F44" s="63" t="s">
-        <v>36</v>
-      </c>
-      <c r="G44" s="78">
-        <f t="shared" si="2"/>
-        <v>0.1</v>
-      </c>
-      <c r="I44" s="31"/>
-      <c r="K44" s="31"/>
-      <c r="M44" s="27">
-        <v>4</v>
-      </c>
-      <c r="N44" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="O44" s="77">
-        <f t="shared" si="4"/>
-        <v>6.6666666666666666E-2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:19" ht="14.25" customHeight="1">
-      <c r="A45" s="57">
-        <v>6</v>
-      </c>
-      <c r="B45" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="C45" s="77">
-        <f t="shared" si="1"/>
-        <v>0.1</v>
-      </c>
-      <c r="E45" s="62">
-        <v>6</v>
-      </c>
-      <c r="F45" s="63" t="s">
-        <v>38</v>
-      </c>
-      <c r="G45" s="78">
-        <f t="shared" si="2"/>
-        <v>0.1</v>
-      </c>
-      <c r="I45" s="31"/>
-      <c r="J45" s="31"/>
-      <c r="K45" s="31"/>
-    </row>
-    <row r="46" spans="1:19" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A46" s="58">
-        <v>6</v>
-      </c>
-      <c r="B46" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="C46" s="77">
-        <f t="shared" si="1"/>
-        <v>0.1</v>
-      </c>
-      <c r="E46" s="62">
-        <v>4</v>
-      </c>
-      <c r="F46" s="63" t="s">
-        <v>37</v>
-      </c>
-      <c r="G46" s="78">
+      <c r="G43" s="48">
         <f t="shared" si="2"/>
         <v>6.6666666666666666E-2</v>
       </c>
-      <c r="I46" s="31"/>
-      <c r="J46" s="31"/>
-      <c r="K46" s="31"/>
+      <c r="I43" s="42">
+        <v>10</v>
+      </c>
+      <c r="J43" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="K43" s="79">
+        <f>$I43/$D$28</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="M43" s="63"/>
+      <c r="N43" s="63"/>
+      <c r="O43" s="75"/>
+      <c r="Q43" s="62"/>
+      <c r="R43" s="62"/>
+      <c r="S43" s="74"/>
+    </row>
+    <row r="44" spans="1:19" ht="14.25" customHeight="1" thickBot="1">
+      <c r="A44" s="62"/>
+      <c r="B44" s="62"/>
+      <c r="C44" s="74"/>
+      <c r="E44" s="60">
+        <v>10</v>
+      </c>
+      <c r="F44" s="61" t="s">
+        <v>34</v>
+      </c>
+      <c r="G44" s="76">
+        <f t="shared" si="2"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I44" s="28"/>
+      <c r="K44" s="28"/>
+      <c r="M44" s="63"/>
+      <c r="N44" s="63"/>
+      <c r="O44" s="75"/>
+    </row>
+    <row r="45" spans="1:19" ht="14.25" customHeight="1">
+      <c r="A45" s="63"/>
+      <c r="B45" s="63"/>
+      <c r="C45" s="75"/>
+      <c r="E45" s="64"/>
+      <c r="F45" s="64"/>
+      <c r="G45" s="77"/>
+      <c r="I45" s="28"/>
+      <c r="J45" s="28"/>
+      <c r="K45" s="28"/>
+    </row>
+    <row r="46" spans="1:19" ht="14.25" customHeight="1" thickBot="1">
+      <c r="A46" s="63"/>
+      <c r="B46" s="63"/>
+      <c r="C46" s="75"/>
+      <c r="E46" s="63"/>
+      <c r="F46" s="63"/>
+      <c r="G46" s="75"/>
+      <c r="I46" s="28"/>
+      <c r="J46" s="28"/>
+      <c r="K46" s="28"/>
     </row>
     <row r="47" spans="1:19" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A47" s="31"/>
-      <c r="B47" s="53"/>
-      <c r="C47" s="31"/>
-      <c r="E47" s="67">
+      <c r="A47" s="80" t="s">
+        <v>44</v>
+      </c>
+      <c r="B47" s="57"/>
+      <c r="C47" s="57"/>
+      <c r="D47" s="57"/>
+      <c r="E47" s="57"/>
+      <c r="F47" s="57"/>
+      <c r="G47" s="57"/>
+      <c r="H47" s="57"/>
+      <c r="I47" s="57"/>
+      <c r="J47" s="57"/>
+      <c r="K47" s="57"/>
+      <c r="L47" s="57"/>
+      <c r="M47" s="57"/>
+      <c r="N47" s="58"/>
+    </row>
+    <row r="48" spans="1:19" ht="14.25" customHeight="1">
+      <c r="A48" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D48" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E48" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F47" s="68" t="s">
-        <v>41</v>
-      </c>
-      <c r="G47" s="78">
-        <f t="shared" si="2"/>
+      <c r="F48" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G48" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H48" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="I48" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="J48" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="K48" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="L48" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="M48" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="N48" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" ht="14.25" customHeight="1">
+      <c r="A49" s="81" t="s">
+        <v>25</v>
+      </c>
+      <c r="B49" s="83">
+        <f>A36/SUM(B28:F28)</f>
+        <v>5.3333333333333337E-2</v>
+      </c>
+      <c r="C49" s="83">
+        <f>SUM(A37,E36)/SUM(B28:F28)</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="D49" s="86">
+        <f>A38/SUM(B28:F28)</f>
+        <v>2.6666666666666668E-2</v>
+      </c>
+      <c r="E49" s="83">
+        <f>SUM(A39,E37)/SUM(B28:F28)</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="F49" s="83">
+        <f>E38/SUM(B28:F28)</f>
+        <v>0.03</v>
+      </c>
+      <c r="G49" s="83">
+        <f>E39/SUM(B28:F28)</f>
+        <v>0.03</v>
+      </c>
+      <c r="H49" s="83">
+        <f>E40/SUM(B28:F28)</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="I49" s="84">
+        <f>SUM(I36,M36,Q36)/SUM(B28:F28)</f>
+        <v>0.10666666666666667</v>
+      </c>
+      <c r="J49" s="84">
+        <f>I37/SUM(B28:F28)</f>
+        <v>5.3333333333333337E-2</v>
+      </c>
+      <c r="K49" s="88">
+        <f>Q37/SUM(B28:F28)</f>
+        <v>0.08</v>
+      </c>
+      <c r="L49" s="84">
+        <f>SUM(I38,M37,Q38)/SUM(B28:F28)</f>
+        <v>9.3333333333333338E-2</v>
+      </c>
+      <c r="M49" s="84">
+        <f>I39/SUM(B28:F28)</f>
+        <v>2.6666666666666668E-2</v>
+      </c>
+      <c r="N49" s="85">
+        <f>SUM(A40,E41,I40,M38,Q39)/SUM(B28:F28)</f>
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" ht="14.25" customHeight="1">
+      <c r="A50" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B50" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C50" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="D50" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E50" s="15"/>
+      <c r="F50" s="15"/>
+      <c r="G50" s="15"/>
+      <c r="H50" s="15"/>
+      <c r="I50" s="15"/>
+      <c r="J50" s="15"/>
+      <c r="K50" s="15"/>
+      <c r="L50" s="15"/>
+      <c r="M50" s="15"/>
+      <c r="N50" s="16"/>
+    </row>
+    <row r="51" spans="1:14" ht="14.25" customHeight="1" thickBot="1">
+      <c r="A51" s="82" t="s">
+        <v>25</v>
+      </c>
+      <c r="B51" s="87">
+        <f>SUM(A41,E42,I41,M39,Q40)/SUM(B28:F28)</f>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="C51" s="87">
+        <f>SUM(A42,E43,I42,M40,Q41)/SUM(B28:F28)</f>
         <v>6.6666666666666666E-2</v>
       </c>
-      <c r="I47" s="31"/>
-      <c r="J47" s="31"/>
-      <c r="K47" s="31"/>
-    </row>
-    <row r="48" spans="1:19" ht="14.25" customHeight="1">
-      <c r="A48" s="31"/>
-      <c r="B48" s="31"/>
-      <c r="C48" s="31"/>
-    </row>
-    <row r="49" ht="14.25" customHeight="1"/>
-    <row r="50" ht="14.25" customHeight="1"/>
-    <row r="51" ht="14.25" customHeight="1"/>
-    <row r="52" ht="14.25" customHeight="1"/>
-    <row r="53" ht="14.25" customHeight="1"/>
-    <row r="54" ht="14.25" customHeight="1"/>
-    <row r="55" ht="14.25" customHeight="1"/>
-    <row r="56" ht="14.25" customHeight="1"/>
-    <row r="57" ht="14.25" customHeight="1"/>
-    <row r="58" ht="14.25" customHeight="1"/>
-    <row r="59" ht="14.25" customHeight="1"/>
-    <row r="60" ht="14.25" customHeight="1"/>
-    <row r="61" ht="14.25" customHeight="1"/>
-    <row r="62" ht="14.25" customHeight="1"/>
-    <row r="63" ht="14.25" customHeight="1"/>
-    <row r="64" ht="14.25" customHeight="1"/>
+      <c r="D51" s="87">
+        <f>SUM(A43,E44,I43,M41,Q42)/SUM(B28:F28)</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="E51" s="18"/>
+      <c r="F51" s="18"/>
+      <c r="G51" s="18"/>
+      <c r="H51" s="18"/>
+      <c r="I51" s="19"/>
+      <c r="J51" s="19"/>
+      <c r="K51" s="20"/>
+      <c r="L51" s="19"/>
+      <c r="M51" s="20"/>
+      <c r="N51" s="21"/>
+    </row>
+    <row r="52" spans="1:14" ht="14.25" customHeight="1"/>
+    <row r="53" spans="1:14" ht="14.25" customHeight="1"/>
+    <row r="54" spans="1:14" ht="14.25" customHeight="1"/>
+    <row r="55" spans="1:14" ht="14.25" customHeight="1"/>
+    <row r="56" spans="1:14" ht="14.25" customHeight="1"/>
+    <row r="57" spans="1:14" ht="14.25" customHeight="1"/>
+    <row r="58" spans="1:14" ht="14.25" customHeight="1"/>
+    <row r="59" spans="1:14" ht="14.25" customHeight="1"/>
+    <row r="60" spans="1:14" ht="14.25" customHeight="1"/>
+    <row r="61" spans="1:14" ht="14.25" customHeight="1"/>
+    <row r="62" spans="1:14" ht="14.25" customHeight="1"/>
+    <row r="63" spans="1:14" ht="14.25" customHeight="1"/>
+    <row r="64" spans="1:14" ht="14.25" customHeight="1"/>
     <row r="65" ht="14.25" customHeight="1"/>
     <row r="66" ht="14.25" customHeight="1"/>
     <row r="67" ht="14.25" customHeight="1"/>
@@ -3689,12 +3774,8 @@
     <row r="1002" ht="14.25" customHeight="1"/>
     <row r="1003" ht="14.25" customHeight="1"/>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="A32:H32"/>
-    <mergeCell ref="A34:C34"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="I34:K34"/>
-    <mergeCell ref="M34:O34"/>
+  <mergeCells count="16">
+    <mergeCell ref="A47:N47"/>
     <mergeCell ref="Q34:S34"/>
     <mergeCell ref="Q11:S11"/>
     <mergeCell ref="A11:C11"/>
@@ -3705,6 +3786,11 @@
     <mergeCell ref="E11:G11"/>
     <mergeCell ref="I11:K11"/>
     <mergeCell ref="M11:O11"/>
+    <mergeCell ref="A32:H32"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="I34:K34"/>
+    <mergeCell ref="M34:O34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>